<commit_message>
Mise à jour site
</commit_message>
<xml_diff>
--- a/prix/prix.xlsx
+++ b/prix/prix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\produits-cimentaires\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD378A1-2BE8-49B5-B92D-45D4C16E55F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5D2CA-721E-4141-B75D-8721D5BFAD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E95DC93-531D-460D-9A06-44397A8920D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="369">
   <si>
     <t>path</t>
   </si>
@@ -977,13 +977,7 @@
     <t>ciments/knauf-ciment-scellement-pr-5kg.png</t>
   </si>
   <si>
-    <t>colles-et-joints-carrelages/mapei-keraflex-blanc-25kg.png</t>
-  </si>
-  <si>
     <t>colles-et-joints-carrelages/mapei-keraflex-blanc-5kg.png</t>
-  </si>
-  <si>
-    <t>colles-et-joints-carrelages/mapei-keraflex-gris-25kg.png</t>
   </si>
   <si>
     <t>colles-et-joints-carrelages/mapei-keraflex-gris-5kg.png</t>
@@ -1694,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065E4AF0-A4F8-4CE3-9E23-EDCEACB756BD}">
   <dimension ref="A1:G332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:A113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1732,7 +1726,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>9</v>
@@ -1752,7 +1746,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>10</v>
@@ -1792,7 +1786,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>41</v>
@@ -1812,7 +1806,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>42</v>
@@ -1832,7 +1826,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>43</v>
@@ -1997,7 +1991,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>52</v>
@@ -2017,7 +2011,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>53</v>
@@ -2127,7 +2121,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>60</v>
@@ -2147,7 +2141,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>61</v>
@@ -2167,7 +2161,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>62</v>
@@ -2247,7 +2241,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>67</v>
@@ -2282,7 +2276,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>69</v>
@@ -2302,7 +2296,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>175</v>
@@ -2322,7 +2316,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>176</v>
@@ -2362,7 +2356,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>178</v>
@@ -2382,7 +2376,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>179</v>
@@ -2402,7 +2396,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>180</v>
@@ -2422,7 +2416,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>181</v>
@@ -2442,7 +2436,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>182</v>
@@ -2482,7 +2476,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>184</v>
@@ -2502,7 +2496,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>185</v>
@@ -2522,7 +2516,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>186</v>
@@ -2578,7 +2572,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>189</v>
@@ -2598,7 +2592,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>190</v>
@@ -2786,7 +2780,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>201</v>
@@ -2806,7 +2800,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>202</v>
@@ -2826,7 +2820,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B62" s="10" t="s">
         <v>203</v>
@@ -2846,7 +2840,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>204</v>
@@ -2866,7 +2860,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>205</v>
@@ -2886,7 +2880,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>206</v>
@@ -2921,7 +2915,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>207</v>
@@ -2941,13 +2935,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>208</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D68" s="3">
         <v>13.16</v>
@@ -2961,13 +2955,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>209</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D69" s="3">
         <v>12.780000000000001</v>
@@ -2981,13 +2975,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>210</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D70" s="3">
         <v>13.16</v>
@@ -3001,13 +2995,13 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>211</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D71" s="3">
         <v>14.14</v>
@@ -3021,13 +3015,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>212</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D72" s="3">
         <v>12.780000000000001</v>
@@ -3041,13 +3035,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>213</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D73" s="3">
         <v>13.200000000000001</v>
@@ -3061,13 +3055,13 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>214</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D74" s="3">
         <v>14.35</v>
@@ -3099,13 +3093,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>216</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D76" s="3">
         <v>24.5</v>
@@ -3119,13 +3113,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>217</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D77" s="3">
         <v>28.22</v>
@@ -3139,13 +3133,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>218</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D78" s="3">
         <v>28.22</v>
@@ -3159,13 +3153,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>219</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D79" s="3">
         <v>28.650000000000002</v>
@@ -3179,13 +3173,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D80" s="3">
         <v>20.3</v>
@@ -3199,13 +3193,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>221</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D81" s="3">
         <v>28.25</v>
@@ -3219,13 +3213,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>222</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D82" s="3">
         <v>25.92</v>
@@ -3239,13 +3233,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D83" s="3">
         <v>27.45</v>
@@ -3259,13 +3253,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>224</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D84" s="3">
         <v>27.41</v>
@@ -3279,13 +3273,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>225</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D85" s="3">
         <v>19.7</v>
@@ -3299,7 +3293,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>226</v>
@@ -3317,13 +3311,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>227</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D87" s="3">
         <v>111.09</v>
@@ -3337,13 +3331,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D88" s="3">
         <v>76.460000000000008</v>
@@ -3357,7 +3351,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>228</v>
@@ -3377,7 +3371,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>229</v>
@@ -3397,7 +3391,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>230</v>
@@ -3417,7 +3411,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>231</v>
@@ -3437,7 +3431,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>232</v>
@@ -3457,7 +3451,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>233</v>
@@ -3477,7 +3471,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>234</v>
@@ -3517,7 +3511,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>236</v>
@@ -3537,7 +3531,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>237</v>
@@ -3557,7 +3551,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>238</v>
@@ -3592,7 +3586,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>240</v>
@@ -3627,7 +3621,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>242</v>
@@ -3821,7 +3815,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B114" s="9" t="s">
         <v>253</v>
@@ -3841,7 +3835,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>254</v>
@@ -3879,7 +3873,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B117" s="9" t="s">
         <v>256</v>
@@ -3899,7 +3893,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B118" s="9" t="s">
         <v>257</v>
@@ -4216,7 +4210,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B136" s="9" t="s">
         <v>275</v>
@@ -4236,7 +4230,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B137" s="9" t="s">
         <v>276</v>
@@ -4256,7 +4250,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B138" s="9" t="s">
         <v>277</v>
@@ -4316,10 +4310,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>287</v>
@@ -4328,7 +4322,7 @@
         <v>17.16</v>
       </c>
       <c r="E141" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F141" s="5">
         <v>5</v>
@@ -4336,10 +4330,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>287</v>
@@ -4348,7 +4342,7 @@
         <v>29.35</v>
       </c>
       <c r="E142" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F142" s="5">
         <v>6</v>
@@ -4356,10 +4350,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>286</v>
@@ -4368,7 +4362,7 @@
         <v>6.01</v>
       </c>
       <c r="E143" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F143" s="5">
         <v>20</v>

</xml_diff>